<commit_message>
Update BOQ view page and L2 view page
</commit_message>
<xml_diff>
--- a/src/assets/tamplate/BOQ_upload_template.xlsx
+++ b/src/assets/tamplate/BOQ_upload_template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pawan Kumar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CEF5F53-9427-4FC4-95FC-DBCF9D74096E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792DBAD7-12FB-4A56-934E-91728884C13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{59ADA35B-B615-4086-857F-279C9099285E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BOQ" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="115">
   <si>
     <t>S No</t>
   </si>
@@ -68,31 +68,320 @@
     <t>SUEPT0001</t>
   </si>
   <si>
-    <t>SUCDG0001</t>
-  </si>
-  <si>
     <t>Nitrogen Injection Fire Protection System (NIFPS) for 40/50MVA Transformers</t>
   </si>
   <si>
-    <t>SUCCH0001</t>
-  </si>
-  <si>
     <t xml:space="preserve">220 kV Lighting Arrestor </t>
   </si>
   <si>
-    <t>SUCMS0001</t>
-  </si>
-  <si>
     <t xml:space="preserve">198 kV, Class III, 10 kA, lightning arrestor along with Surge monitor </t>
   </si>
   <si>
-    <t>SUCNE0001</t>
-  </si>
-  <si>
     <t>220 kV Isolator/ Disconnecting Switches</t>
   </si>
   <si>
-    <t>On line DGA monitoring for each transformer working on spectroscopy method.</t>
+    <t>SUE400001</t>
+  </si>
+  <si>
+    <t>SUEON0001</t>
+  </si>
+  <si>
+    <t>On line DGA monitoring for each transformer working on spectroscopy
+method.</t>
+  </si>
+  <si>
+    <t>SUENI0001</t>
+  </si>
+  <si>
+    <t>SUE220004</t>
+  </si>
+  <si>
+    <t>SUE190001</t>
+  </si>
+  <si>
+    <t>SUE220005</t>
+  </si>
+  <si>
+    <t>SUECE0001</t>
+  </si>
+  <si>
+    <t>Centre break tandom isolator (Double Break) 245kV, 2000A, 40kA for 3Sec.</t>
+  </si>
+  <si>
+    <t>SUECE0002</t>
+  </si>
+  <si>
+    <t>Centre break isolator with one Earth switch (Double Break) 245kV, 2000A, 40kA for 3Sec.</t>
+  </si>
+  <si>
+    <t>SUECE0003</t>
+  </si>
+  <si>
+    <t>Centre break tandom isolator with one Earth switch (Double Break) 245kV, 2000A, 40kA for 3Sec.</t>
+  </si>
+  <si>
+    <t>SUECE0004</t>
+  </si>
+  <si>
+    <t>Centre break isolator with two Earth switch (Double Break) 245kV, 2000A, 40kA for 3Sec.</t>
+  </si>
+  <si>
+    <t>SUE220006</t>
+  </si>
+  <si>
+    <t>220 kV SF6 Circuit Breaker</t>
+  </si>
+  <si>
+    <t>SUE220007</t>
+  </si>
+  <si>
+    <t>220 kV, 2000A, 40 kA for 3 sec, 3 pole SF6 type circuit breaker</t>
+  </si>
+  <si>
+    <t>SUE220008</t>
+  </si>
+  <si>
+    <t>220 kV Current Transformer</t>
+  </si>
+  <si>
+    <t>SUE240001</t>
+  </si>
+  <si>
+    <t>245kV, 40kA Current transformer (1-PH)</t>
+  </si>
+  <si>
+    <t>SUE240002</t>
+  </si>
+  <si>
+    <t>245kV, Current transformer (1-PH) for OPTCL</t>
+  </si>
+  <si>
+    <t>SUE240003</t>
+  </si>
+  <si>
+    <t>245kV Capacitive voltage transformer (1-PH) for OPTCL</t>
+  </si>
+  <si>
+    <t>SUECT0001</t>
+  </si>
+  <si>
+    <t>CT for grid metering</t>
+  </si>
+  <si>
+    <t>SUE220009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">220 kV Potential Transformer </t>
+  </si>
+  <si>
+    <t>SUE240004</t>
+  </si>
+  <si>
+    <t>245kV Potential transformer (1-PH)</t>
+  </si>
+  <si>
+    <t>PT for grid metering</t>
+  </si>
+  <si>
+    <t>220 kV Bus Post Insulator</t>
+  </si>
+  <si>
+    <t>SUESU0001</t>
+  </si>
+  <si>
+    <t>Summation metering- check metering voltage selection scheme and other associated auxiliaries related to metering</t>
+  </si>
+  <si>
+    <t>SUE220010</t>
+  </si>
+  <si>
+    <t>220 kV Erection Hardware</t>
+  </si>
+  <si>
+    <t>SUEHA0001</t>
+  </si>
+  <si>
+    <t>Hardware Fittings</t>
+  </si>
+  <si>
+    <t>SUEDI0001</t>
+  </si>
+  <si>
+    <t>Disc Insulator</t>
+  </si>
+  <si>
+    <t>SUECO0010</t>
+  </si>
+  <si>
+    <t>Conductor</t>
+  </si>
+  <si>
+    <t>SUEIP0001</t>
+  </si>
+  <si>
+    <t>IPS tube</t>
+  </si>
+  <si>
+    <t>SUE330003</t>
+  </si>
+  <si>
+    <t>33 kV Circuit Breaker</t>
+  </si>
+  <si>
+    <t>SUE330004</t>
+  </si>
+  <si>
+    <t>3 pole, 33 kV, 1600 A, 31.5 kA for 3 sec. SC, outdoor type Vacuum circuit breaker</t>
+  </si>
+  <si>
+    <t>SUE330005</t>
+  </si>
+  <si>
+    <t>33 kV Isolator</t>
+  </si>
+  <si>
+    <t>SUEWI0001</t>
+  </si>
+  <si>
+    <t>With One Earth switch Centre break, 33kV, 1600A, 31.5kA 3Sec (1-PH)</t>
+  </si>
+  <si>
+    <t>SUEWI0002</t>
+  </si>
+  <si>
+    <t>With Two Earth switch Centre break, 33kV, 1600A, 31.5kA 3Sec (1-PH)</t>
+  </si>
+  <si>
+    <t>SUEOU0001</t>
+  </si>
+  <si>
+    <t>Outdoor type, 33kV class CT for 3 poles with 5 nos. cores (3 nos. PS class, 1 no. 5P20 and 1 no. Class 1.0)</t>
+  </si>
+  <si>
+    <t>SUE120001</t>
+  </si>
+  <si>
+    <t>1200 Amps,5 Core,  120%</t>
+  </si>
+  <si>
+    <t>SUE800001</t>
+  </si>
+  <si>
+    <t>800 Amps,5 Core, 150%</t>
+  </si>
+  <si>
+    <t>SUE330006</t>
+  </si>
+  <si>
+    <t>33 kV Potential Transformer</t>
+  </si>
+  <si>
+    <t>SUE330007</t>
+  </si>
+  <si>
+    <t>33kV/110V/√3/110V/√3 Potential transformers - 0.2S</t>
+  </si>
+  <si>
+    <t>SUE330008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33 kV Lighting Arrestor </t>
+  </si>
+  <si>
+    <t>SUECL0001</t>
+  </si>
+  <si>
+    <t>Class III, 10 KA LA with Surge Monitor</t>
+  </si>
+  <si>
+    <t>SUE330009</t>
+  </si>
+  <si>
+    <t>33 kV Bus Post Insulator</t>
+  </si>
+  <si>
+    <t>SUE330010</t>
+  </si>
+  <si>
+    <t>33 kV Erection Hardware</t>
+  </si>
+  <si>
+    <t>SUEFI0001</t>
+  </si>
+  <si>
+    <t>Fibre optic Ground wire (OPGW )</t>
+  </si>
+  <si>
+    <t>SUEDR0001</t>
+  </si>
+  <si>
+    <t>Dry Type distribution Transformers-Indoor</t>
+  </si>
+  <si>
+    <t>SUE330011</t>
+  </si>
+  <si>
+    <t>33 kV/433 V, 630 kVA (Minimum) AN transformers along with incoming 33 kV indoor isolators</t>
+  </si>
+  <si>
+    <t>SUE330012</t>
+  </si>
+  <si>
+    <t>33kV isoltaor for above LT transformer</t>
+  </si>
+  <si>
+    <t>SUELT0001</t>
+  </si>
+  <si>
+    <t>LT Panel</t>
+  </si>
+  <si>
+    <t>SUE410001</t>
+  </si>
+  <si>
+    <t>415 V Main switchboard</t>
+  </si>
+  <si>
+    <t>SUEMO0001</t>
+  </si>
+  <si>
+    <t>Motor Control System (MCC). MCC shall comprise of two incomers, bus coupler and required number of outgoing feeders with 20 % spare</t>
+  </si>
+  <si>
+    <t>SUELT0002</t>
+  </si>
+  <si>
+    <t>LT Squirrel Cage AC Induction Motor, 415 V, 3-ph, 50 Hz, AC</t>
+  </si>
+  <si>
+    <t>SUELO0001</t>
+  </si>
+  <si>
+    <t>Local Control Station (LCS)</t>
+  </si>
+  <si>
+    <t>SUE220011</t>
+  </si>
+  <si>
+    <t>220 V, 200AH ( minimum) Plante Battery bank</t>
+  </si>
+  <si>
+    <t>SUE220012</t>
+  </si>
+  <si>
+    <t>220 V Charger twin type Float cum boost</t>
+  </si>
+  <si>
+    <t>SUE480001</t>
+  </si>
+  <si>
+    <t>48Volt 200 AH- VRLA</t>
+  </si>
+  <si>
+    <t>SUE480002</t>
+  </si>
+  <si>
+    <t>48 Volt, 40 A twin type Float cum boost</t>
   </si>
 </sst>
 </file>
@@ -506,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA6B386-46A5-4CF6-BA2C-DF9D9AC77B71}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +835,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>7</v>
@@ -557,19 +846,16 @@
       <c r="E2" s="3">
         <v>2</v>
       </c>
-      <c r="F2" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
@@ -577,28 +863,22 @@
       <c r="E3" s="3">
         <v>2</v>
       </c>
-      <c r="F3" s="3">
-        <v>12</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>1.2</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="3">
         <v>2</v>
-      </c>
-      <c r="F4" s="3">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -606,19 +886,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -626,19 +900,16 @@
         <v>2.1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="3">
         <v>12</v>
-      </c>
-      <c r="F6" s="3">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -646,10 +917,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>8</v>
@@ -657,7 +928,888 @@
       <c r="E7" s="3">
         <v>0</v>
       </c>
-      <c r="F7" s="3">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>5</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>5.1999999999999993</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>5.2999999999999989</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>5.3999999999999986</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>6.1999999999999993</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>7</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>8</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>9</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>9.1</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>9.2999999999999989</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>9.3999999999999986</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>10</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>10.1</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>11</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>11.1</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>11.2</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>12</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>12.1</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>13</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>13.1</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>14</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>14.1</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>15</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>16</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>16.200000000000003</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>16.300000000000004</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>16.400000000000006</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>17</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>18</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>18.200000000000003</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>19</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>20</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>21</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>22</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>23</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>24</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>25</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>26</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BOQ item update UI done with all function
</commit_message>
<xml_diff>
--- a/src/assets/tamplate/BOQ_upload_template.xlsx
+++ b/src/assets/tamplate/BOQ_upload_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pawan Kumar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GEPDEC-INFRA\src\assets\tamplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792DBAD7-12FB-4A56-934E-91728884C13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6ABDDA-D2CC-4B42-A09E-9D3B7CC260A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{59ADA35B-B615-4086-857F-279C9099285E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="116">
   <si>
     <t>S No</t>
   </si>
@@ -382,6 +382,9 @@
   </si>
   <si>
     <t>48 Volt, 40 A twin type Float cum boost</t>
+  </si>
+  <si>
+    <t>Freight Charges</t>
   </si>
 </sst>
 </file>
@@ -452,15 +455,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,22 +795,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA6B386-46A5-4CF6-BA2C-DF9D9AC77B71}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="76.85546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="80.28515625" style="4" customWidth="1"/>
     <col min="4" max="5" width="10.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -829,8 +828,11 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -847,14 +849,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -864,7 +866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1.2000000000000002</v>
       </c>
@@ -881,7 +883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -895,7 +897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2.1</v>
       </c>
@@ -912,7 +914,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -929,7 +931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>3.1</v>
       </c>
@@ -946,7 +948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>3.2</v>
       </c>
@@ -963,7 +965,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>3.3</v>
       </c>
@@ -980,7 +982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>3.4</v>
       </c>
@@ -997,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>4</v>
       </c>
@@ -1014,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>4.0999999999999996</v>
       </c>
@@ -1031,7 +1033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>5</v>
       </c>
@@ -1048,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>5.0999999999999996</v>
       </c>
@@ -1065,7 +1067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>5.1999999999999993</v>
       </c>
@@ -1815,5 +1817,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>